<commit_message>
updates to subtype in te_metadata_table_final.csv & notes on embl_repbase_mapping.xlsx
</commit_message>
<xml_diff>
--- a/misc/metadata/embl_repbase_mapping.xlsx
+++ b/misc/metadata/embl_repbase_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shunhua/git/transposons/misc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casey/github/transposons/misc/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50167E3F-BD10-314B-88FA-87C81B1D9580}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3036587-7F64-3046-A6B8-412F2352009A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22400" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="embl_repbase_match" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="type_conversion" sheetId="4" r:id="rId3"/>
     <sheet name="wicker" sheetId="3" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dmel_table!$A$1:$Q$127</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">embl_repbase_match!$A$1:$T$180</definedName>
@@ -29,6 +26,82 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Casey Bergman</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{F3BF82D0-70F9-8645-98C0-23D126C6016B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Casey Bergman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>this column is wrong</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J139" authorId="0" shapeId="0" xr:uid="{602F704B-D4C4-2542-82D7-525559EC2C7F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Casey Bergman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>this is wrong</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4739" uniqueCount="1227">
   <si>
@@ -3717,7 +3790,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3859,6 +3932,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -4271,48 +4357,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>DNA</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>LTR</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>LINE</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>RC</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>foldback_element</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>DNA</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4609,11 +4653,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1080" topLeftCell="A111" activePane="bottomLeft"/>
+      <selection activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4626,7 +4672,7 @@
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
     <col min="7" max="7" width="30.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="29.83203125" customWidth="1"/>
     <col min="11" max="11" width="24" customWidth="1"/>
     <col min="12" max="12" width="22.5" customWidth="1"/>
@@ -15466,6 +15512,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>